<commit_message>
Updated forms of reports
</commit_message>
<xml_diff>
--- a/Reports/Отчет - ПодТипыПроектов.xlsx
+++ b/Reports/Отчет - ПодТипыПроектов.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D174AC07-4600-4D28-821B-C90AFDE9EC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DD41C8-A769-49ED-A9BC-33F5024D5702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="_ВозможныеСписки">Настройки!$A$1:$A$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ИсходныеДанные!$A$1:$AT$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ИсходныеДанные!$A$1:$AW$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Отчет!$C$8:$AB$50</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="113">
   <si>
     <t>I</t>
   </si>
@@ -389,6 +389,15 @@
   </si>
   <si>
     <t>boss_email</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>Portfolio_Month</t>
   </si>
 </sst>
 </file>
@@ -398,12 +407,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -871,126 +888,130 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный 3 2" xfId="3" xr:uid="{527D8C01-00B1-4577-8938-D759098F6077}"/>
+    <cellStyle name="Процентный 2" xfId="2" xr:uid="{8B21E1AC-585C-4E8E-A74D-FCA78ED460FA}"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1378,10 +1399,10 @@
       <c r="B1" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="33"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="15">
         <f t="shared" ref="E1:AB1" ca="1" si="0">SUM(E6:E50)</f>
         <v>0</v>
@@ -1484,10 +1505,10 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>61</v>
       </c>
       <c r="E2" s="13">
@@ -1597,23 +1618,23 @@
       <c r="A4" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="23" t="str">
+      <c r="B4" s="22" t="str">
         <f>VLOOKUP(УникальныеСписки!A1,Настройки!A1:D50,3,FALSE)</f>
         <v>AH</v>
       </c>
-      <c r="C4" s="22" t="str">
+      <c r="C4" s="21" t="str">
         <f>VLOOKUP(УникальныеСписки!A1,Настройки!A1:D20,3,FALSE)</f>
         <v>AH</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="43" t="str">
+      <c r="E4" s="39" t="str">
         <f>VLOOKUP(УникальныеСписки!A1,Настройки!A1:D50,4,FALSE)</f>
         <v>AL</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="23">
+      <c r="F4" s="40"/>
+      <c r="G4" s="22">
         <f>ROW(B9)-2</f>
         <v>7</v>
       </c>
@@ -1623,41 +1644,41 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="36"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="45"/>
+      <c r="S5" s="45"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="45"/>
+      <c r="X5" s="45"/>
+      <c r="Y5" s="45"/>
+      <c r="Z5" s="45"/>
+      <c r="AA5" s="45"/>
+      <c r="AB5" s="38"/>
       <c r="AC5" s="4"/>
     </row>
     <row r="6" spans="1:29" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1665,57 +1686,57 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="35" t="s">
+      <c r="B6" s="42"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="35" t="s">
+      <c r="F6" s="38"/>
+      <c r="G6" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="35" t="s">
+      <c r="H6" s="38"/>
+      <c r="I6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="36"/>
-      <c r="K6" s="35" t="s">
+      <c r="J6" s="38"/>
+      <c r="K6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="36"/>
-      <c r="M6" s="35" t="s">
+      <c r="L6" s="38"/>
+      <c r="M6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="36"/>
-      <c r="O6" s="35" t="s">
+      <c r="N6" s="38"/>
+      <c r="O6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="35" t="s">
+      <c r="P6" s="38"/>
+      <c r="Q6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="36"/>
-      <c r="S6" s="35" t="s">
+      <c r="R6" s="38"/>
+      <c r="S6" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="36"/>
-      <c r="U6" s="35" t="s">
+      <c r="T6" s="38"/>
+      <c r="U6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="V6" s="36"/>
-      <c r="W6" s="35" t="s">
+      <c r="V6" s="38"/>
+      <c r="W6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="X6" s="36"/>
-      <c r="Y6" s="35" t="s">
+      <c r="X6" s="38"/>
+      <c r="Y6" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="35" t="s">
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="AB6" s="36"/>
+      <c r="AB6" s="38"/>
       <c r="AC6" s="4"/>
     </row>
     <row r="7" spans="1:29" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1723,9 +1744,9 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="42"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="11" t="s">
         <v>17</v>
       </c>
@@ -1805,9 +1826,9 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
       <c r="G8" s="8"/>
@@ -1839,15 +1860,15 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="19">
         <f t="array" aca="1" ref="B9" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C9" s="34" t="str" cm="1">
+      <c r="C9" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">_xlfn.XLOOKUP($B9,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D9" s="30" t="str">
+      <c r="D9" s="29" t="str">
         <f t="array" aca="1" ref="D9" ca="1">_xlfn.XLOOKUP($B9,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -1954,15 +1975,15 @@
         <f t="shared" ref="A10:A50" ca="1" si="2">IF(D10="","delete","")</f>
         <v>delete</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="20">
         <f t="array" aca="1" ref="B10" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="34" t="str" cm="1">
+      <c r="C10" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">_xlfn.XLOOKUP($B10,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D10" s="30" t="str">
+      <c r="D10" s="29" t="str">
         <f t="array" aca="1" ref="D10" ca="1">_xlfn.XLOOKUP($B10,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -2069,15 +2090,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="20">
         <f t="array" aca="1" ref="B11" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C11" s="34" t="str" cm="1">
+      <c r="C11" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">_xlfn.XLOOKUP($B11,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D11" s="30" t="str">
+      <c r="D11" s="29" t="str">
         <f t="array" aca="1" ref="D11" ca="1">_xlfn.XLOOKUP($B11,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -2184,15 +2205,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <f t="array" aca="1" ref="B12" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="34" t="str" cm="1">
+      <c r="C12" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">_xlfn.XLOOKUP($B12,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D12" s="30" t="str">
+      <c r="D12" s="29" t="str">
         <f t="array" aca="1" ref="D12" ca="1">_xlfn.XLOOKUP($B12,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -2299,15 +2320,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="20">
         <f t="array" aca="1" ref="B13" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C13" s="34" t="str" cm="1">
+      <c r="C13" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">_xlfn.XLOOKUP($B13,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D13" s="30" t="str">
+      <c r="D13" s="29" t="str">
         <f t="array" aca="1" ref="D13" ca="1">_xlfn.XLOOKUP($B13,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -2414,15 +2435,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <f t="array" aca="1" ref="B14" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="34" t="str" cm="1">
+      <c r="C14" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">_xlfn.XLOOKUP($B14,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D14" s="30" t="str">
+      <c r="D14" s="29" t="str">
         <f t="array" aca="1" ref="D14" ca="1">_xlfn.XLOOKUP($B14,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -2529,15 +2550,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="20">
         <f t="array" aca="1" ref="B15" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="34" t="str" cm="1">
+      <c r="C15" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">_xlfn.XLOOKUP($B15,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D15" s="30" t="str">
+      <c r="D15" s="29" t="str">
         <f t="array" aca="1" ref="D15" ca="1">_xlfn.XLOOKUP($B15,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -2644,15 +2665,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <f t="array" aca="1" ref="B16" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="34" t="str" cm="1">
+      <c r="C16" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">_xlfn.XLOOKUP($B16,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D16" s="30" t="str">
+      <c r="D16" s="29" t="str">
         <f t="array" aca="1" ref="D16" ca="1">_xlfn.XLOOKUP($B16,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -2759,15 +2780,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="20">
         <f t="array" aca="1" ref="B17" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C17" s="34" t="str" cm="1">
+      <c r="C17" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">_xlfn.XLOOKUP($B17,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D17" s="30" t="str">
+      <c r="D17" s="29" t="str">
         <f t="array" aca="1" ref="D17" ca="1">_xlfn.XLOOKUP($B17,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -2874,15 +2895,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="20">
         <f t="array" aca="1" ref="B18" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C18" s="34" t="str" cm="1">
+      <c r="C18" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">_xlfn.XLOOKUP($B18,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D18" s="30" t="str">
+      <c r="D18" s="29" t="str">
         <f t="array" aca="1" ref="D18" ca="1">_xlfn.XLOOKUP($B18,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -2989,15 +3010,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="20">
         <f t="array" aca="1" ref="B19" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C19" s="34" t="str" cm="1">
+      <c r="C19" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">_xlfn.XLOOKUP($B19,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D19" s="30" t="str">
+      <c r="D19" s="29" t="str">
         <f t="array" aca="1" ref="D19" ca="1">_xlfn.XLOOKUP($B19,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -3104,15 +3125,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="20">
         <f t="array" aca="1" ref="B20" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C20" s="34" t="str" cm="1">
+      <c r="C20" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">_xlfn.XLOOKUP($B20,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D20" s="30" t="str">
+      <c r="D20" s="29" t="str">
         <f t="array" aca="1" ref="D20" ca="1">_xlfn.XLOOKUP($B20,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -3219,15 +3240,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="20">
         <f t="array" aca="1" ref="B21" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C21" s="34" t="str" cm="1">
+      <c r="C21" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">_xlfn.XLOOKUP($B21,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D21" s="30" t="str">
+      <c r="D21" s="29" t="str">
         <f t="array" aca="1" ref="D21" ca="1">_xlfn.XLOOKUP($B21,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -3334,15 +3355,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="20">
         <f t="array" aca="1" ref="B22" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="34" t="str" cm="1">
+      <c r="C22" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">_xlfn.XLOOKUP($B22,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D22" s="30" t="str">
+      <c r="D22" s="29" t="str">
         <f t="array" aca="1" ref="D22" ca="1">_xlfn.XLOOKUP($B22,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -3449,15 +3470,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="20">
         <f t="array" aca="1" ref="B23" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C23" s="34" t="str" cm="1">
+      <c r="C23" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C23" ca="1">_xlfn.XLOOKUP($B23,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D23" s="30" t="str">
+      <c r="D23" s="29" t="str">
         <f t="array" aca="1" ref="D23" ca="1">_xlfn.XLOOKUP($B23,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -3564,15 +3585,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B24" s="20">
         <f t="array" aca="1" ref="B24" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C24" s="34" t="str" cm="1">
+      <c r="C24" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C24" ca="1">_xlfn.XLOOKUP($B24,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D24" s="30" t="str">
+      <c r="D24" s="29" t="str">
         <f t="array" aca="1" ref="D24" ca="1">_xlfn.XLOOKUP($B24,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -3679,15 +3700,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="20">
         <f t="array" aca="1" ref="B25" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C25" s="34" t="str" cm="1">
+      <c r="C25" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C25" ca="1">_xlfn.XLOOKUP($B25,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D25" s="30" t="str">
+      <c r="D25" s="29" t="str">
         <f t="array" aca="1" ref="D25" ca="1">_xlfn.XLOOKUP($B25,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -3794,15 +3815,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="20">
         <f t="array" aca="1" ref="B26" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C26" s="34" t="str" cm="1">
+      <c r="C26" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C26" ca="1">_xlfn.XLOOKUP($B26,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D26" s="30" t="str">
+      <c r="D26" s="29" t="str">
         <f t="array" aca="1" ref="D26" ca="1">_xlfn.XLOOKUP($B26,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -3909,15 +3930,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B27" s="20">
         <f t="array" aca="1" ref="B27" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C27" s="34" t="str" cm="1">
+      <c r="C27" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C27" ca="1">_xlfn.XLOOKUP($B27,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D27" s="30" t="str">
+      <c r="D27" s="29" t="str">
         <f t="array" aca="1" ref="D27" ca="1">_xlfn.XLOOKUP($B27,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -4024,15 +4045,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="20">
         <f t="array" aca="1" ref="B28" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C28" s="34" t="str" cm="1">
+      <c r="C28" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C28" ca="1">_xlfn.XLOOKUP($B28,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D28" s="30" t="str">
+      <c r="D28" s="29" t="str">
         <f t="array" aca="1" ref="D28" ca="1">_xlfn.XLOOKUP($B28,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -4139,15 +4160,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B29" s="21">
+      <c r="B29" s="20">
         <f t="array" aca="1" ref="B29" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C29" s="34" t="str" cm="1">
+      <c r="C29" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C29" ca="1">_xlfn.XLOOKUP($B29,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D29" s="30" t="str">
+      <c r="D29" s="29" t="str">
         <f t="array" aca="1" ref="D29" ca="1">_xlfn.XLOOKUP($B29,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -4254,15 +4275,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B30" s="21">
+      <c r="B30" s="20">
         <f t="array" aca="1" ref="B30" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C30" s="34" t="str" cm="1">
+      <c r="C30" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C30" ca="1">_xlfn.XLOOKUP($B30,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D30" s="30" t="str">
+      <c r="D30" s="29" t="str">
         <f t="array" aca="1" ref="D30" ca="1">_xlfn.XLOOKUP($B30,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -4369,15 +4390,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="20">
         <f t="array" aca="1" ref="B31" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C31" s="34" t="str" cm="1">
+      <c r="C31" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C31" ca="1">_xlfn.XLOOKUP($B31,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D31" s="30" t="str">
+      <c r="D31" s="29" t="str">
         <f t="array" aca="1" ref="D31" ca="1">_xlfn.XLOOKUP($B31,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -4484,15 +4505,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B32" s="21">
+      <c r="B32" s="20">
         <f t="array" aca="1" ref="B32" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C32" s="34" t="str" cm="1">
+      <c r="C32" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C32" ca="1">_xlfn.XLOOKUP($B32,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D32" s="30" t="str">
+      <c r="D32" s="29" t="str">
         <f t="array" aca="1" ref="D32" ca="1">_xlfn.XLOOKUP($B32,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -4599,15 +4620,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B33" s="21">
+      <c r="B33" s="20">
         <f t="array" aca="1" ref="B33" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C33" s="34" t="str" cm="1">
+      <c r="C33" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C33" ca="1">_xlfn.XLOOKUP($B33,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D33" s="30" t="str">
+      <c r="D33" s="29" t="str">
         <f t="array" aca="1" ref="D33" ca="1">_xlfn.XLOOKUP($B33,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -4714,15 +4735,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B34" s="21">
+      <c r="B34" s="20">
         <f t="array" aca="1" ref="B34" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C34" s="34" t="str" cm="1">
+      <c r="C34" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C34" ca="1">_xlfn.XLOOKUP($B34,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D34" s="30" t="str">
+      <c r="D34" s="29" t="str">
         <f t="array" aca="1" ref="D34" ca="1">_xlfn.XLOOKUP($B34,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -4829,15 +4850,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B35" s="21">
+      <c r="B35" s="20">
         <f t="array" aca="1" ref="B35" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C35" s="34" t="str" cm="1">
+      <c r="C35" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C35" ca="1">_xlfn.XLOOKUP($B35,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D35" s="30" t="str">
+      <c r="D35" s="29" t="str">
         <f t="array" aca="1" ref="D35" ca="1">_xlfn.XLOOKUP($B35,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -4944,15 +4965,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B36" s="21">
+      <c r="B36" s="20">
         <f t="array" aca="1" ref="B36" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C36" s="34" t="str" cm="1">
+      <c r="C36" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C36" ca="1">_xlfn.XLOOKUP($B36,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D36" s="30" t="str">
+      <c r="D36" s="29" t="str">
         <f t="array" aca="1" ref="D36" ca="1">_xlfn.XLOOKUP($B36,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -5059,15 +5080,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B37" s="21">
+      <c r="B37" s="20">
         <f t="array" aca="1" ref="B37" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C37" s="34" t="str" cm="1">
+      <c r="C37" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C37" ca="1">_xlfn.XLOOKUP($B37,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D37" s="30" t="str">
+      <c r="D37" s="29" t="str">
         <f t="array" aca="1" ref="D37" ca="1">_xlfn.XLOOKUP($B37,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -5174,15 +5195,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B38" s="21">
+      <c r="B38" s="20">
         <f t="array" aca="1" ref="B38" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C38" s="34" t="str" cm="1">
+      <c r="C38" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C38" ca="1">_xlfn.XLOOKUP($B38,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D38" s="30" t="str">
+      <c r="D38" s="29" t="str">
         <f t="array" aca="1" ref="D38" ca="1">_xlfn.XLOOKUP($B38,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -5289,15 +5310,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B39" s="21">
+      <c r="B39" s="20">
         <f t="array" aca="1" ref="B39" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C39" s="34" t="str" cm="1">
+      <c r="C39" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C39" ca="1">_xlfn.XLOOKUP($B39,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D39" s="30" t="str">
+      <c r="D39" s="29" t="str">
         <f t="array" aca="1" ref="D39" ca="1">_xlfn.XLOOKUP($B39,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -5404,15 +5425,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B40" s="21">
+      <c r="B40" s="20">
         <f t="array" aca="1" ref="B40" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C40" s="34" t="str" cm="1">
+      <c r="C40" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C40" ca="1">_xlfn.XLOOKUP($B40,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D40" s="30" t="str">
+      <c r="D40" s="29" t="str">
         <f t="array" aca="1" ref="D40" ca="1">_xlfn.XLOOKUP($B40,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -5519,15 +5540,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B41" s="21">
+      <c r="B41" s="20">
         <f t="array" aca="1" ref="B41" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C41" s="34" t="str" cm="1">
+      <c r="C41" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C41" ca="1">_xlfn.XLOOKUP($B41,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D41" s="30" t="str">
+      <c r="D41" s="29" t="str">
         <f t="array" aca="1" ref="D41" ca="1">_xlfn.XLOOKUP($B41,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -5634,15 +5655,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B42" s="21">
+      <c r="B42" s="20">
         <f t="array" aca="1" ref="B42" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C42" s="34" t="str" cm="1">
+      <c r="C42" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C42" ca="1">_xlfn.XLOOKUP($B42,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D42" s="30" t="str">
+      <c r="D42" s="29" t="str">
         <f t="array" aca="1" ref="D42" ca="1">_xlfn.XLOOKUP($B42,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -5749,15 +5770,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B43" s="21">
+      <c r="B43" s="20">
         <f t="array" aca="1" ref="B43" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C43" s="34" t="str" cm="1">
+      <c r="C43" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C43" ca="1">_xlfn.XLOOKUP($B43,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D43" s="30" t="str">
+      <c r="D43" s="29" t="str">
         <f t="array" aca="1" ref="D43" ca="1">_xlfn.XLOOKUP($B43,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -5864,15 +5885,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B44" s="21">
+      <c r="B44" s="20">
         <f t="array" aca="1" ref="B44" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C44" s="34" t="str" cm="1">
+      <c r="C44" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C44" ca="1">_xlfn.XLOOKUP($B44,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D44" s="30" t="str">
+      <c r="D44" s="29" t="str">
         <f t="array" aca="1" ref="D44" ca="1">_xlfn.XLOOKUP($B44,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -5979,15 +6000,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B45" s="21">
+      <c r="B45" s="20">
         <f t="array" aca="1" ref="B45" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C45" s="34" t="str" cm="1">
+      <c r="C45" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C45" ca="1">_xlfn.XLOOKUP($B45,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D45" s="30" t="str">
+      <c r="D45" s="29" t="str">
         <f t="array" aca="1" ref="D45" ca="1">_xlfn.XLOOKUP($B45,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -6094,15 +6115,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B46" s="21">
+      <c r="B46" s="20">
         <f t="array" aca="1" ref="B46" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C46" s="34" t="str" cm="1">
+      <c r="C46" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C46" ca="1">_xlfn.XLOOKUP($B46,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D46" s="30" t="str">
+      <c r="D46" s="29" t="str">
         <f t="array" aca="1" ref="D46" ca="1">_xlfn.XLOOKUP($B46,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -6209,15 +6230,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B47" s="21">
+      <c r="B47" s="20">
         <f t="array" aca="1" ref="B47" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C47" s="34" t="str" cm="1">
+      <c r="C47" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C47" ca="1">_xlfn.XLOOKUP($B47,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D47" s="30" t="str">
+      <c r="D47" s="29" t="str">
         <f t="array" aca="1" ref="D47" ca="1">_xlfn.XLOOKUP($B47,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -6324,15 +6345,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B48" s="21">
+      <c r="B48" s="20">
         <f t="array" aca="1" ref="B48" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C48" s="34" t="str" cm="1">
+      <c r="C48" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C48" ca="1">_xlfn.XLOOKUP($B48,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D48" s="30" t="str">
+      <c r="D48" s="29" t="str">
         <f t="array" aca="1" ref="D48" ca="1">_xlfn.XLOOKUP($B48,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -6439,15 +6460,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B49" s="21">
+      <c r="B49" s="20">
         <f t="array" aca="1" ref="B49" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C49" s="34" t="str" cm="1">
+      <c r="C49" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C49" ca="1">_xlfn.XLOOKUP($B49,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D49" s="30" t="str">
+      <c r="D49" s="29" t="str">
         <f t="array" aca="1" ref="D49" ca="1">_xlfn.XLOOKUP($B49,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -6554,15 +6575,15 @@
         <f t="shared" ca="1" si="2"/>
         <v>delete</v>
       </c>
-      <c r="B50" s="24">
+      <c r="B50" s="23">
         <f t="array" aca="1" ref="B50" ca="1">INDIRECT("УникальныеСписки!A"&amp;ROW()-$G$4)</f>
         <v>0</v>
       </c>
-      <c r="C50" s="34" t="str" cm="1">
+      <c r="C50" s="32" t="str" cm="1">
         <f t="array" aca="1" ref="C50" ca="1">_xlfn.XLOOKUP($B50,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",C$4)),"",0,1)</f>
         <v/>
       </c>
-      <c r="D50" s="30" t="str">
+      <c r="D50" s="29" t="str">
         <f t="array" aca="1" ref="D50" ca="1">_xlfn.XLOOKUP($B50,INDIRECT(SUBSTITUTE("ИсходныеДанные!$где$2:$где$50000","где",$B$4)),INDIRECT(SUBSTITUTE("ИсходныеДанные!$что$2:$что$50000","что",D$4)),"",0,1)</f>
         <v/>
       </c>
@@ -6699,11 +6720,6 @@
   </sheetData>
   <autoFilter ref="C8:AB50" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="17">
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B5:B8"/>
     <mergeCell ref="W6:X6"/>
     <mergeCell ref="E5:AB5"/>
     <mergeCell ref="M6:N6"/>
@@ -6716,6 +6732,11 @@
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="U6:V6"/>
     <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:AB2">
     <cfRule type="expression" dxfId="2" priority="6">
@@ -6740,12 +6761,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:AT1"/>
+  <dimension ref="A1:AW1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C5" sqref="C5:C8"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:AW1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6791,148 +6812,157 @@
     <col min="39" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="P1" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="R1" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="S1" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="T1" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="U1" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="V1" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="W1" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="X1" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Y1" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="Z1" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AA1" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AB1" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AC1" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AD1" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AE1" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="AF1" s="31" t="s">
+      <c r="AF1" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="AG1" s="31" t="s">
+      <c r="AG1" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" s="31" t="s">
+      <c r="AH1" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="AI1" s="31" t="s">
+      <c r="AI1" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="AJ1" s="31" t="s">
+      <c r="AJ1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="AK1" s="31" t="s">
+      <c r="AK1" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="AL1" s="31" t="s">
+      <c r="AL1" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="AM1" s="31" t="s">
+      <c r="AM1" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="AN1" s="31" t="s">
+      <c r="AN1" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="AO1" s="31" t="s">
+      <c r="AO1" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="AP1" s="31" t="s">
+      <c r="AP1" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="AQ1" s="31" t="s">
+      <c r="AQ1" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="AR1" s="31" t="s">
+      <c r="AR1" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="AS1" s="31" t="s">
+      <c r="AS1" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="AT1" s="31" t="s">
+      <c r="AT1" s="47" t="s">
         <v>109</v>
+      </c>
+      <c r="AU1" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="AV1" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="AW1" s="47" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AT1" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
+  <autoFilter ref="A1:AW1" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
 </worksheet>
@@ -6949,17 +6979,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68" style="25" customWidth="1"/>
+    <col min="1" max="1" width="68" style="24" customWidth="1"/>
     <col min="2" max="2" width="59.7109375" style="18" customWidth="1"/>
     <col min="3" max="5" width="9.140625" style="18" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="26" t="str">
+      <c r="B1" s="25" t="str">
         <f>VLOOKUP(A1,Настройки!A1:B37,2,FALSE)</f>
         <v>ПодТип проекта</v>
       </c>

</xml_diff>

<commit_message>
Updated settings in all files.
</commit_message>
<xml_diff>
--- a/Reports/Отчет - ПодТипыПроектов.xlsx
+++ b/Reports/Отчет - ПодТипыПроектов.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DD41C8-A769-49ED-A9BC-33F5024D5702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1C9A6B-6B28-411D-8211-453959BD40E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ИсходныеДанные!$A$1:$AW$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Отчет!$C$8:$AB$50</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="174">
   <si>
     <t>I</t>
   </si>
@@ -398,6 +398,189 @@
   </si>
   <si>
     <t>Portfolio_Month</t>
+  </si>
+  <si>
+    <t>IS_Service_type</t>
+  </si>
+  <si>
+    <t>IS_Service_type_Month</t>
+  </si>
+  <si>
+    <t>IS_Product_type</t>
+  </si>
+  <si>
+    <t>IS_Product_type_Month</t>
+  </si>
+  <si>
+    <t>Pdr_Proj</t>
+  </si>
+  <si>
+    <t>Pdr_Proj_Month</t>
+  </si>
+  <si>
+    <t>Proj_Pdr</t>
+  </si>
+  <si>
+    <t>Proj_Pdr_Month</t>
+  </si>
+  <si>
+    <t>FN_Month</t>
+  </si>
+  <si>
+    <t>UHCost_KV1</t>
+  </si>
+  <si>
+    <t>UMCost_KV1</t>
+  </si>
+  <si>
+    <t>UHCost_KV2</t>
+  </si>
+  <si>
+    <t>UMCost_KV2</t>
+  </si>
+  <si>
+    <t>UHCost_KV3</t>
+  </si>
+  <si>
+    <t>UMCost_KV3</t>
+  </si>
+  <si>
+    <t>UHCost_KV4</t>
+  </si>
+  <si>
+    <t>UMCost_KV4</t>
+  </si>
+  <si>
+    <t>ISDogName</t>
+  </si>
+  <si>
+    <t>Тип сервиса (ИСУ, КИС, ЛИС, ПУ, ..)</t>
+  </si>
+  <si>
+    <t>AX</t>
+  </si>
+  <si>
+    <t>AY</t>
+  </si>
+  <si>
+    <t>Тип системы (SAP, БК, ЛИМС, MES,…)</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>Группировка Подразделение+Проект</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>Группировка Проект+Подразделение</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Портфель проектов</t>
+  </si>
+  <si>
+    <t>AV</t>
+  </si>
+  <si>
+    <t>AW</t>
+  </si>
+  <si>
+    <t>Признак отправлять сообщение лично или в общей массе</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Почтовый адрес пользователя</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Почтовый адрес руководителя данного пользователя</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>Доходный договор</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>Функциональное направление (или подразделение)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>Часовая ставка в 1-м квартале</t>
+  </si>
+  <si>
+    <t>Месячная ставка в 1-м квартале</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>Часовая ставка во 2-м квартале</t>
+  </si>
+  <si>
+    <t>BH</t>
+  </si>
+  <si>
+    <t>Месячная ставка во 2-м квартале</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>Часовая ставка в 3-м квартале</t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>Месячная ставка в 3-м квартале</t>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>Часовая ставка в 4-м квартале</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>Месячная ставка в 4-м квартале</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>Название ИС из договора</t>
+  </si>
+  <si>
+    <t>BO</t>
   </si>
 </sst>
 </file>
@@ -971,6 +1154,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -983,10 +1180,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -996,16 +1189,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1629,11 +1812,11 @@
       <c r="D4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="39" t="str">
+      <c r="E4" s="43" t="str">
         <f>VLOOKUP(УникальныеСписки!A1,Настройки!A1:D50,4,FALSE)</f>
         <v>AL</v>
       </c>
-      <c r="F4" s="40"/>
+      <c r="F4" s="44"/>
       <c r="G4" s="22">
         <f>ROW(B9)-2</f>
         <v>7</v>
@@ -1644,41 +1827,41 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="45"/>
-      <c r="X5" s="45"/>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45"/>
-      <c r="AB5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="38"/>
+      <c r="Y5" s="38"/>
+      <c r="Z5" s="38"/>
+      <c r="AA5" s="38"/>
+      <c r="AB5" s="36"/>
       <c r="AC5" s="4"/>
     </row>
     <row r="6" spans="1:29" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1686,57 +1869,57 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37" t="s">
+      <c r="B6" s="46"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="37" t="s">
+      <c r="F6" s="36"/>
+      <c r="G6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="37" t="s">
+      <c r="H6" s="36"/>
+      <c r="I6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="37" t="s">
+      <c r="J6" s="36"/>
+      <c r="K6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="38"/>
-      <c r="M6" s="37" t="s">
+      <c r="L6" s="36"/>
+      <c r="M6" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="N6" s="38"/>
-      <c r="O6" s="37" t="s">
+      <c r="N6" s="36"/>
+      <c r="O6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="37" t="s">
+      <c r="P6" s="36"/>
+      <c r="Q6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="38"/>
-      <c r="S6" s="37" t="s">
+      <c r="R6" s="36"/>
+      <c r="S6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="T6" s="38"/>
-      <c r="U6" s="37" t="s">
+      <c r="T6" s="36"/>
+      <c r="U6" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="V6" s="38"/>
-      <c r="W6" s="37" t="s">
+      <c r="V6" s="36"/>
+      <c r="W6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="X6" s="38"/>
-      <c r="Y6" s="37" t="s">
+      <c r="X6" s="36"/>
+      <c r="Y6" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="Z6" s="38"/>
-      <c r="AA6" s="37" t="s">
+      <c r="Z6" s="36"/>
+      <c r="AA6" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="AB6" s="38"/>
+      <c r="AB6" s="36"/>
       <c r="AC6" s="4"/>
     </row>
     <row r="7" spans="1:29" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1744,9 +1927,9 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="36"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="11" t="s">
         <v>17</v>
       </c>
@@ -1826,7 +2009,7 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B8" s="43"/>
+      <c r="B8" s="47"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="8"/>
@@ -6720,6 +6903,11 @@
   </sheetData>
   <autoFilter ref="C8:AB50" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="17">
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B5:B8"/>
     <mergeCell ref="W6:X6"/>
     <mergeCell ref="E5:AB5"/>
     <mergeCell ref="M6:N6"/>
@@ -6732,11 +6920,6 @@
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="U6:V6"/>
     <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:AB2">
     <cfRule type="expression" dxfId="2" priority="6">
@@ -6761,12 +6944,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:AW1"/>
+  <dimension ref="A1:BO1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C5" sqref="C5:C8"/>
-      <selection pane="bottomLeft" sqref="A1:AW1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6812,153 +6995,207 @@
     <col min="39" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="46" t="s">
+      <c r="L1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="S1" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="46" t="s">
+      <c r="V1" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="46" t="s">
+      <c r="W1" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="X1" s="46" t="s">
+      <c r="X1" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="46" t="s">
+      <c r="Y1" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="Z1" s="46" t="s">
+      <c r="Z1" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="46" t="s">
+      <c r="AA1" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="AB1" s="46" t="s">
+      <c r="AB1" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="AC1" s="46" t="s">
+      <c r="AC1" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="AD1" s="46" t="s">
+      <c r="AD1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="AE1" s="46" t="s">
+      <c r="AE1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="AF1" s="47" t="s">
+      <c r="AF1" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="AG1" s="47" t="s">
+      <c r="AG1" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" s="47" t="s">
+      <c r="AH1" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="AI1" s="47" t="s">
+      <c r="AI1" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="AJ1" s="47" t="s">
+      <c r="AJ1" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="AK1" s="47" t="s">
+      <c r="AK1" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="AL1" s="47" t="s">
+      <c r="AL1" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="AM1" s="47" t="s">
+      <c r="AM1" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="AN1" s="47" t="s">
+      <c r="AN1" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="AO1" s="47" t="s">
+      <c r="AO1" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="AP1" s="47" t="s">
+      <c r="AP1" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="AQ1" s="47" t="s">
+      <c r="AQ1" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="AR1" s="47" t="s">
+      <c r="AR1" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="AS1" s="47" t="s">
+      <c r="AS1" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="AT1" s="47" t="s">
+      <c r="AT1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="AU1" s="47" t="s">
+      <c r="AU1" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="AV1" s="47" t="s">
+      <c r="AV1" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="AW1" s="47" t="s">
+      <c r="AW1" s="34" t="s">
         <v>112</v>
+      </c>
+      <c r="AX1" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="AY1" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="AZ1" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="BA1" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="BB1" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC1" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="BD1" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="BE1" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF1" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="BG1" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="BH1" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="BI1" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="BJ1" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="BK1" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="BL1" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="BM1" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="BN1" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="BO1" s="34" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -7008,10 +7245,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Лист3"/>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7230,6 +7467,246 @@
         <v>49</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="18"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" s="18"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D27" s="18"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="18"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" s="18"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="18"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D33" s="18"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" s="18"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Report files updated:   - fixed cost calculation errors;   - updated list of used data columns;   - updated pointers to column names (settings).
</commit_message>
<xml_diff>
--- a/Reports/Отчет - ПодТипыПроектов.xlsx
+++ b/Reports/Отчет - ПодТипыПроектов.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1C9A6B-6B28-411D-8211-453959BD40E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821624FB-B505-4D2D-B05A-EA00643DD31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ИсходныеДанные!$A$1:$AW$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Отчет!$C$8:$AB$50</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual" calcCompleted="0"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -56,15 +56,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="174">
-  <si>
-    <t>I</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="142">
   <si>
     <t>G</t>
-  </si>
-  <si>
-    <t>E</t>
   </si>
   <si>
     <t>Идентификатор
@@ -123,9 +117,6 @@
     <t>Подразделение</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -144,9 +135,6 @@
     <t>Функциональное направление + проект</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -156,9 +144,6 @@
     <t>Функциональное направление + проект + ФИО</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
@@ -168,9 +153,6 @@
     <t>Подразделение + ФИО</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>Q</t>
   </si>
   <si>
@@ -180,9 +162,6 @@
     <t>Подразделение + ФИО + проект</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -192,9 +171,6 @@
     <t>Менеджер проекта + проект</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>U</t>
   </si>
   <si>
@@ -204,18 +180,12 @@
     <t>Менеджер проекта + проект + ФИО</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
     <t>ShortProject</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -252,9 +222,6 @@
     <t>Pdr_User_ProjType_Month</t>
   </si>
   <si>
-    <t>AD</t>
-  </si>
-  <si>
     <t>AE</t>
   </si>
   <si>
@@ -264,9 +231,6 @@
     <t>ProjectSubTypeDescription</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>ProjectSubType</t>
   </si>
   <si>
@@ -285,13 +249,7 @@
     <t>Подразделение + ФИО + ПодТип Проекта</t>
   </si>
   <si>
-    <t>AJ</t>
-  </si>
-  <si>
     <t>AK</t>
-  </si>
-  <si>
-    <t>AH</t>
   </si>
   <si>
     <t>Под
@@ -457,78 +415,48 @@
     <t>Тип сервиса (ИСУ, КИС, ЛИС, ПУ, ..)</t>
   </si>
   <si>
-    <t>AX</t>
-  </si>
-  <si>
     <t>AY</t>
   </si>
   <si>
     <t>Тип системы (SAP, БК, ЛИМС, MES,…)</t>
   </si>
   <si>
-    <t>AZ</t>
-  </si>
-  <si>
     <t>BA</t>
   </si>
   <si>
     <t>Группировка Подразделение+Проект</t>
   </si>
   <si>
-    <t>BB</t>
-  </si>
-  <si>
     <t>BC</t>
   </si>
   <si>
     <t>Группировка Проект+Подразделение</t>
   </si>
   <si>
-    <t>BD</t>
-  </si>
-  <si>
     <t>BE</t>
   </si>
   <si>
     <t>Портфель проектов</t>
   </si>
   <si>
-    <t>AV</t>
-  </si>
-  <si>
     <t>AW</t>
   </si>
   <si>
     <t>Признак отправлять сообщение лично или в общей массе</t>
   </si>
   <si>
-    <t>AR</t>
-  </si>
-  <si>
     <t>Почтовый адрес пользователя</t>
   </si>
   <si>
-    <t>AS</t>
-  </si>
-  <si>
     <t>Почтовый адрес руководителя данного пользователя</t>
   </si>
   <si>
-    <t>AT</t>
-  </si>
-  <si>
     <t>Доходный договор</t>
   </si>
   <si>
-    <t>AU</t>
-  </si>
-  <si>
     <t>Функциональное направление (или подразделение)</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>BF</t>
   </si>
   <si>
@@ -538,49 +466,25 @@
     <t>Месячная ставка в 1-м квартале</t>
   </si>
   <si>
-    <t>BG</t>
-  </si>
-  <si>
     <t>Часовая ставка во 2-м квартале</t>
   </si>
   <si>
-    <t>BH</t>
-  </si>
-  <si>
     <t>Месячная ставка во 2-м квартале</t>
   </si>
   <si>
-    <t>BI</t>
-  </si>
-  <si>
     <t>Часовая ставка в 3-м квартале</t>
   </si>
   <si>
-    <t>BJ</t>
-  </si>
-  <si>
     <t>Месячная ставка в 3-м квартале</t>
   </si>
   <si>
-    <t>BK</t>
-  </si>
-  <si>
     <t>Часовая ставка в 4-м квартале</t>
   </si>
   <si>
-    <t>BL</t>
-  </si>
-  <si>
     <t>Месячная ставка в 4-м квартале</t>
   </si>
   <si>
-    <t>BM</t>
-  </si>
-  <si>
     <t>Название ИС из договора</t>
-  </si>
-  <si>
-    <t>BO</t>
   </si>
 </sst>
 </file>
@@ -1580,10 +1484,10 @@
         <v/>
       </c>
       <c r="B1" s="16" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D1" s="31"/>
       <c r="E1" s="15">
@@ -1689,10 +1593,10 @@
         <v/>
       </c>
       <c r="C2" s="28" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E2" s="13">
         <f t="shared" ref="E2:AB2" ca="1" si="1">SUBTOTAL(9,E6:E51)</f>
@@ -1799,7 +1703,7 @@
     </row>
     <row r="4" spans="1:29" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B4" s="22" t="str">
         <f>VLOOKUP(УникальныеСписки!A1,Настройки!A1:D50,3,FALSE)</f>
@@ -1810,7 +1714,7 @@
         <v>AH</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="43" t="str">
         <f>VLOOKUP(УникальныеСписки!A1,Настройки!A1:D50,4,FALSE)</f>
@@ -1828,16 +1732,16 @@
         <v/>
       </c>
       <c r="B5" s="45" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
@@ -1873,51 +1777,51 @@
       <c r="C6" s="40"/>
       <c r="D6" s="42"/>
       <c r="E6" s="35" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" s="36"/>
       <c r="G6" s="35" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H6" s="36"/>
       <c r="I6" s="35" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J6" s="36"/>
       <c r="K6" s="35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L6" s="36"/>
       <c r="M6" s="35" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N6" s="36"/>
       <c r="O6" s="35" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P6" s="36"/>
       <c r="Q6" s="35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R6" s="36"/>
       <c r="S6" s="35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="T6" s="36"/>
       <c r="U6" s="35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="V6" s="36"/>
       <c r="W6" s="35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="X6" s="36"/>
       <c r="Y6" s="35" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Z6" s="36"/>
       <c r="AA6" s="35" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AB6" s="36"/>
       <c r="AC6" s="4"/>
@@ -1931,76 +1835,76 @@
       <c r="C7" s="40"/>
       <c r="D7" s="42"/>
       <c r="E7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="R7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="T7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="U7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="V7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="X7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="Y7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Z7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AA7" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AB7" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC7" s="4"/>
     </row>
@@ -6949,7 +6853,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C5" sqref="C5:C8"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6992,210 +6896,239 @@
     <col min="36" max="36" width="21.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="28.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="32.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="18"/>
+    <col min="39" max="39" width="13.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18" style="18" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13" style="18" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="22.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="68" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="R1" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="T1" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="V1" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="AB1" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="AC1" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="33" t="s">
+      <c r="AD1" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE1" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="AG1" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH1" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="33" t="s">
+      <c r="AI1" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="AJ1" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK1" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="33" t="s">
+      <c r="AL1" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="P1" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="R1" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="S1" s="33" t="s">
+      <c r="AM1" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="U1" s="33" t="s">
+      <c r="AN1" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="V1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="W1" s="33" t="s">
+      <c r="AO1" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="X1" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y1" s="33" t="s">
+      <c r="AP1" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="Z1" s="33" t="s">
+      <c r="AQ1" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="AA1" s="33" t="s">
+      <c r="AR1" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="AB1" s="33" t="s">
+      <c r="AS1" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="AC1" s="33" t="s">
+      <c r="AT1" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="AD1" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE1" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF1" s="34" t="s">
+      <c r="AU1" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="AG1" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH1" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI1" s="34" t="s">
+      <c r="AV1" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="AJ1" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK1" s="34" t="s">
+      <c r="AW1" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="AL1" s="34" t="s">
+      <c r="AX1" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="AM1" s="34" t="s">
+      <c r="AY1" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="AZ1" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="BA1" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="AN1" s="34" t="s">
+      <c r="BB1" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="AO1" s="34" t="s">
+      <c r="BC1" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="AP1" s="34" t="s">
+      <c r="BD1" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="AQ1" s="34" t="s">
+      <c r="BE1" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="AR1" s="34" t="s">
+      <c r="BF1" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="AS1" s="34" t="s">
+      <c r="BG1" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="AT1" s="34" t="s">
+      <c r="BH1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="AU1" s="34" t="s">
+      <c r="BI1" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="AV1" s="34" t="s">
+      <c r="BJ1" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="AW1" s="34" t="s">
+      <c r="BK1" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="AX1" s="34" t="s">
+      <c r="BL1" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="AY1" s="34" t="s">
+      <c r="BM1" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="AZ1" s="34" t="s">
+      <c r="BN1" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="BA1" s="34" t="s">
+      <c r="BO1" s="34" t="s">
         <v>116</v>
-      </c>
-      <c r="BB1" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC1" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="BD1" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="BE1" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="BF1" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="BG1" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="BH1" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="BI1" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="BJ1" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="BK1" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="BL1" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="BM1" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="BN1" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="BO1" s="34" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -7224,7 +7157,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B1" s="25" t="str">
         <f>VLOOKUP(A1,Настройки!A1:B37,2,FALSE)</f>
@@ -7248,7 +7181,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D34"/>
+      <selection activeCell="C1" sqref="C1:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7259,451 +7192,485 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="C1" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A1,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>D</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A2,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>E</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>51</v>
+        <v>2</v>
+      </c>
+      <c r="C3" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A3,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>X</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>1</v>
+        <v>47</v>
+      </c>
+      <c r="C4" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A4,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>G</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>68</v>
+        <v>58</v>
+      </c>
+      <c r="C5" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A5,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>H</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>77</v>
+        <v>58</v>
+      </c>
+      <c r="C6" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A6,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>AH</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="C7" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A7,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>AD</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>75</v>
+        <v>62</v>
+      </c>
+      <c r="C8" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A8,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>AJ</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A9,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>I</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A10,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>L</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="C11" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A11,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>N</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="C12" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A12,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>P</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="C13" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A13,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>R</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="C14" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A14,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>T</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="C15" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A15,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>V</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>132</v>
+        <v>117</v>
+      </c>
+      <c r="C16" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A16,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>AX</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>135</v>
+        <v>119</v>
+      </c>
+      <c r="C17" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A17,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>AZ</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>138</v>
+        <v>121</v>
+      </c>
+      <c r="C18" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A18,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BB</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>141</v>
+        <v>123</v>
+      </c>
+      <c r="C19" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A19,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BD</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>144</v>
+        <v>125</v>
+      </c>
+      <c r="C20" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A20,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>AV</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>147</v>
+        <v>127</v>
+      </c>
+      <c r="C21" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A21,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>AR</v>
       </c>
       <c r="D21" s="18"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>149</v>
+        <v>128</v>
+      </c>
+      <c r="C22" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A22,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>AS</v>
       </c>
       <c r="D22" s="18"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>151</v>
+        <v>129</v>
+      </c>
+      <c r="C23" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A23,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>AT</v>
       </c>
       <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>153</v>
+        <v>130</v>
+      </c>
+      <c r="C24" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A24,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>AU</v>
       </c>
       <c r="D24" s="18"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>155</v>
+        <v>131</v>
+      </c>
+      <c r="C25" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A25,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>C</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>156</v>
+        <v>133</v>
+      </c>
+      <c r="C26" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A26,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BG</v>
       </c>
       <c r="D26" s="18"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>159</v>
+        <v>134</v>
+      </c>
+      <c r="C27" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A27,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BH</v>
       </c>
       <c r="D27" s="18"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>161</v>
+        <v>135</v>
+      </c>
+      <c r="C28" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A28,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BI</v>
       </c>
       <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>163</v>
+        <v>136</v>
+      </c>
+      <c r="C29" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A29,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BJ</v>
       </c>
       <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>165</v>
+        <v>137</v>
+      </c>
+      <c r="C30" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A30,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BK</v>
       </c>
       <c r="D30" s="18"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>167</v>
+        <v>138</v>
+      </c>
+      <c r="C31" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A31,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BL</v>
       </c>
       <c r="D31" s="18"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>169</v>
+        <v>139</v>
+      </c>
+      <c r="C32" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A32,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BM</v>
       </c>
       <c r="D32" s="18"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>171</v>
+        <v>140</v>
+      </c>
+      <c r="C33" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A33,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BN</v>
       </c>
       <c r="D33" s="18"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>173</v>
+        <v>141</v>
+      </c>
+      <c r="C34" s="18" t="str">
+        <f>SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A34,ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <v>BO</v>
       </c>
       <c r="D34" s="18"/>
     </row>

</xml_diff>

<commit_message>
Fixed error in formulas.
</commit_message>
<xml_diff>
--- a/Reports/Отчет - ПодТипыПроектов.xlsx
+++ b/Reports/Отчет - ПодТипыПроектов.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708DB0E7-764E-4CE3-889B-92B178215F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0852BC10-3B2F-4604-9444-447892F91CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,9 +13,6 @@
     <sheet name="УникальныеСписки" sheetId="4" r:id="rId3"/>
     <sheet name="Настройки" sheetId="2" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_ВозможныеСписки">Настройки!$A$1:$A$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ИсходныеДанные!$A$1:$CC$1</definedName>
@@ -1100,14 +1097,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1120,6 +1109,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1129,6 +1122,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1202,271 +1199,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Отчет"/>
-      <sheetName val="ИсходныеДанные"/>
-      <sheetName val="УникальныеСписки"/>
-      <sheetName val="Настройки"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>FDate</v>
-          </cell>
-          <cell r="B1" t="str">
-            <v>Month</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>FN</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>Division</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>User</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>Project</v>
-          </cell>
-          <cell r="G1" t="str">
-            <v>ProjectType</v>
-          </cell>
-          <cell r="H1" t="str">
-            <v>ProjectSubType</v>
-          </cell>
-          <cell r="I1" t="str">
-            <v>ProjectManager</v>
-          </cell>
-          <cell r="J1" t="str">
-            <v>PlanFTE</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v>FactFTE</v>
-          </cell>
-          <cell r="L1" t="str">
-            <v>FN_Proj</v>
-          </cell>
-          <cell r="M1" t="str">
-            <v>FN_Proj_Month</v>
-          </cell>
-          <cell r="N1" t="str">
-            <v>FN_Proj_User</v>
-          </cell>
-          <cell r="O1" t="str">
-            <v>FN_Proj_User_Month</v>
-          </cell>
-          <cell r="P1" t="str">
-            <v>Pdr_User</v>
-          </cell>
-          <cell r="Q1" t="str">
-            <v>Pdr_User_Month</v>
-          </cell>
-          <cell r="R1" t="str">
-            <v>Pdr_User_Proj</v>
-          </cell>
-          <cell r="S1" t="str">
-            <v>Pdr_User_Proj_Month</v>
-          </cell>
-          <cell r="T1" t="str">
-            <v>ProjMang_Proj</v>
-          </cell>
-          <cell r="U1" t="str">
-            <v>ProjMang_Proj_Month</v>
-          </cell>
-          <cell r="V1" t="str">
-            <v>ProjMang_Proj_User</v>
-          </cell>
-          <cell r="W1" t="str">
-            <v>ProjMang_Proj_User_Month</v>
-          </cell>
-          <cell r="X1" t="str">
-            <v>ShortProject</v>
-          </cell>
-          <cell r="Y1" t="str">
-            <v>ShortProject_Month</v>
-          </cell>
-          <cell r="Z1" t="str">
-            <v>Division_Month</v>
-          </cell>
-          <cell r="AA1" t="str">
-            <v>User_Month</v>
-          </cell>
-          <cell r="AB1" t="str">
-            <v>ProjectType_Month</v>
-          </cell>
-          <cell r="AC1" t="str">
-            <v>ProjectManager_Month</v>
-          </cell>
-          <cell r="AD1" t="str">
-            <v>Pdr_User_ProjType</v>
-          </cell>
-          <cell r="AE1" t="str">
-            <v>Pdr_User_ProjType_Month</v>
-          </cell>
-          <cell r="AF1" t="str">
-            <v>FactHours</v>
-          </cell>
-          <cell r="AG1" t="str">
-            <v>ProjectTypeDescription</v>
-          </cell>
-          <cell r="AH1" t="str">
-            <v>ProjectSubTypeDescription</v>
-          </cell>
-          <cell r="AI1" t="str">
-            <v>ProjectSubType_Month</v>
-          </cell>
-          <cell r="AJ1" t="str">
-            <v>Pdr_User_ProjSubType</v>
-          </cell>
-          <cell r="AK1" t="str">
-            <v>Pdr_User_ProjSubType_Month</v>
-          </cell>
-          <cell r="AL1" t="str">
-            <v>ProjectSubTypeDescription_Month</v>
-          </cell>
-          <cell r="AM1" t="str">
-            <v>pVacasia</v>
-          </cell>
-          <cell r="AN1" t="str">
-            <v>Northern</v>
-          </cell>
-          <cell r="AO1" t="str">
-            <v>JustUserName</v>
-          </cell>
-          <cell r="AP1" t="str">
-            <v>UserHourCost</v>
-          </cell>
-          <cell r="AQ1" t="str">
-            <v>UserMonthCost</v>
-          </cell>
-          <cell r="AR1" t="str">
-            <v>Personal_email</v>
-          </cell>
-          <cell r="AS1" t="str">
-            <v>user_email</v>
-          </cell>
-          <cell r="AT1" t="str">
-            <v>boss_email</v>
-          </cell>
-          <cell r="AU1" t="str">
-            <v>Contract</v>
-          </cell>
-          <cell r="AV1" t="str">
-            <v>Portfolio</v>
-          </cell>
-          <cell r="AW1" t="str">
-            <v>Portfolio_Month</v>
-          </cell>
-          <cell r="AX1" t="str">
-            <v>IS_Service_type</v>
-          </cell>
-          <cell r="AY1" t="str">
-            <v>IS_Service_type_Month</v>
-          </cell>
-          <cell r="AZ1" t="str">
-            <v>IS_Product_type</v>
-          </cell>
-          <cell r="BA1" t="str">
-            <v>IS_Product_type_Month</v>
-          </cell>
-          <cell r="BB1" t="str">
-            <v>Pdr_Proj</v>
-          </cell>
-          <cell r="BC1" t="str">
-            <v>Pdr_Proj_Month</v>
-          </cell>
-          <cell r="BD1" t="str">
-            <v>Proj_Pdr</v>
-          </cell>
-          <cell r="BE1" t="str">
-            <v>Proj_Pdr_Month</v>
-          </cell>
-          <cell r="BF1" t="str">
-            <v>FN_Month</v>
-          </cell>
-          <cell r="BG1" t="str">
-            <v>UHCost_KV1</v>
-          </cell>
-          <cell r="BH1" t="str">
-            <v>UMCost_KV1</v>
-          </cell>
-          <cell r="BI1" t="str">
-            <v>UHCost_KV2</v>
-          </cell>
-          <cell r="BJ1" t="str">
-            <v>UMCost_KV2</v>
-          </cell>
-          <cell r="BK1" t="str">
-            <v>UHCost_KV3</v>
-          </cell>
-          <cell r="BL1" t="str">
-            <v>UMCost_KV3</v>
-          </cell>
-          <cell r="BM1" t="str">
-            <v>UHCost_KV4</v>
-          </cell>
-          <cell r="BN1" t="str">
-            <v>UMCost_KV4</v>
-          </cell>
-          <cell r="BO1" t="str">
-            <v>ISDogName</v>
-          </cell>
-          <cell r="BP1" t="str">
-            <v>SumUserFHours</v>
-          </cell>
-          <cell r="BQ1" t="str">
-            <v>SumUserFactFTE</v>
-          </cell>
-          <cell r="BR1" t="str">
-            <v>SumUserFactFTEUR</v>
-          </cell>
-          <cell r="BS1" t="str">
-            <v>HourTo1FTE</v>
-          </cell>
-          <cell r="BT1" t="str">
-            <v>HourTo1FTE_Math</v>
-          </cell>
-          <cell r="BU1" t="str">
-            <v>_________________</v>
-          </cell>
-          <cell r="BV1" t="str">
-            <v>_________________</v>
-          </cell>
-          <cell r="BW1" t="str">
-            <v>_________________</v>
-          </cell>
-          <cell r="BX1" t="str">
-            <v>_________________</v>
-          </cell>
-          <cell r="BY1" t="str">
-            <v>_________________</v>
-          </cell>
-          <cell r="BZ1" t="str">
-            <v>_________________</v>
-          </cell>
-          <cell r="CA1" t="str">
-            <v>_________________</v>
-          </cell>
-          <cell r="CB1" t="str">
-            <v>_________________</v>
-          </cell>
-          <cell r="CC1" t="str">
-            <v>_________________</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2017,11 +1749,11 @@
       <c r="D4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="43" t="str">
+      <c r="E4" s="41" t="str">
         <f ca="1">VLOOKUP(УникальныеСписки!A1,Настройки!A1:D50,4,FALSE)</f>
         <v>AL</v>
       </c>
-      <c r="F4" s="44"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="22">
         <f>ROW(B9)-2</f>
         <v>7</v>
@@ -2032,41 +1764,41 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="38"/>
-      <c r="X5" s="38"/>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="36"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="47"/>
+      <c r="W5" s="47"/>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="40"/>
       <c r="AC5" s="4"/>
     </row>
     <row r="6" spans="1:29" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2074,57 +1806,57 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="35" t="s">
+      <c r="B6" s="44"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="35" t="s">
+      <c r="F6" s="40"/>
+      <c r="G6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="35" t="s">
+      <c r="H6" s="40"/>
+      <c r="I6" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="36"/>
-      <c r="K6" s="35" t="s">
+      <c r="J6" s="40"/>
+      <c r="K6" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="36"/>
-      <c r="M6" s="35" t="s">
+      <c r="L6" s="40"/>
+      <c r="M6" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="36"/>
-      <c r="O6" s="35" t="s">
+      <c r="N6" s="40"/>
+      <c r="O6" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="35" t="s">
+      <c r="P6" s="40"/>
+      <c r="Q6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="36"/>
-      <c r="S6" s="35" t="s">
+      <c r="R6" s="40"/>
+      <c r="S6" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="36"/>
-      <c r="U6" s="35" t="s">
+      <c r="T6" s="40"/>
+      <c r="U6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="V6" s="36"/>
-      <c r="W6" s="35" t="s">
+      <c r="V6" s="40"/>
+      <c r="W6" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="X6" s="36"/>
-      <c r="Y6" s="35" t="s">
+      <c r="X6" s="40"/>
+      <c r="Y6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="35" t="s">
+      <c r="Z6" s="40"/>
+      <c r="AA6" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="AB6" s="36"/>
+      <c r="AB6" s="40"/>
       <c r="AC6" s="4"/>
     </row>
     <row r="7" spans="1:29" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2132,9 +1864,9 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="42"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="11" t="s">
         <v>15</v>
       </c>
@@ -2214,7 +1946,7 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B8" s="47"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="8"/>
@@ -7108,11 +6840,6 @@
   </sheetData>
   <autoFilter ref="C8:AB50" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="17">
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B5:B8"/>
     <mergeCell ref="W6:X6"/>
     <mergeCell ref="E5:AB5"/>
     <mergeCell ref="M6:N6"/>
@@ -7125,6 +6852,11 @@
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="U6:V6"/>
     <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B5:B8"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:AB2">
     <cfRule type="expression" dxfId="2" priority="6">
@@ -7529,9 +7261,7 @@
   <sheetPr codeName="Лист3"/>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D39"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7547,7 +7277,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A1,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A1,INDIRECT("ИсходныеДанные!$A$1:$DD$1"),0,1),4),1,"")</f>
         <v>D</v>
       </c>
       <c r="D1" s="18" t="s">
@@ -7562,7 +7292,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A2,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ref="C2:C39" ca="1" si="0">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A2,INDIRECT("ИсходныеДанные!$A$1:$DD$1"),0,1),4),1,"")</f>
         <v>E</v>
       </c>
       <c r="D2" s="18" t="s">
@@ -7577,7 +7307,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A3,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>X</v>
       </c>
       <c r="D3" s="18" t="s">
@@ -7592,7 +7322,7 @@
         <v>47</v>
       </c>
       <c r="C4" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A4,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>G</v>
       </c>
       <c r="D4" s="18" t="s">
@@ -7607,7 +7337,7 @@
         <v>58</v>
       </c>
       <c r="C5" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A5,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>H</v>
       </c>
       <c r="D5" s="18" t="s">
@@ -7622,7 +7352,7 @@
         <v>58</v>
       </c>
       <c r="C6" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A6,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>AH</v>
       </c>
       <c r="D6" s="18" t="s">
@@ -7637,7 +7367,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A7,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>AD</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -7652,7 +7382,7 @@
         <v>62</v>
       </c>
       <c r="C8" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A8,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>AJ</v>
       </c>
       <c r="D8" s="18" t="s">
@@ -7667,7 +7397,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A9,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>I</v>
       </c>
       <c r="D9" s="18" t="s">
@@ -7682,7 +7412,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A10,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>L</v>
       </c>
       <c r="D10" s="18" t="s">
@@ -7697,7 +7427,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A11,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>N</v>
       </c>
       <c r="D11" s="18" t="s">
@@ -7712,7 +7442,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A12,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>P</v>
       </c>
       <c r="D12" s="18" t="s">
@@ -7727,7 +7457,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A13,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>R</v>
       </c>
       <c r="D13" s="18" t="s">
@@ -7742,7 +7472,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A14,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>T</v>
       </c>
       <c r="D14" s="18" t="s">
@@ -7757,7 +7487,7 @@
         <v>39</v>
       </c>
       <c r="C15" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A15,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>V</v>
       </c>
       <c r="D15" s="18" t="s">
@@ -7772,7 +7502,7 @@
         <v>117</v>
       </c>
       <c r="C16" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A16,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>AX</v>
       </c>
       <c r="D16" s="18" t="s">
@@ -7787,7 +7517,7 @@
         <v>119</v>
       </c>
       <c r="C17" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A17,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>AZ</v>
       </c>
       <c r="D17" s="18" t="s">
@@ -7802,7 +7532,7 @@
         <v>121</v>
       </c>
       <c r="C18" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A18,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BB</v>
       </c>
       <c r="D18" s="18" t="s">
@@ -7817,7 +7547,7 @@
         <v>123</v>
       </c>
       <c r="C19" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A19,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BD</v>
       </c>
       <c r="D19" s="18" t="s">
@@ -7832,7 +7562,7 @@
         <v>125</v>
       </c>
       <c r="C20" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A20,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>AV</v>
       </c>
       <c r="D20" s="18" t="s">
@@ -7847,7 +7577,7 @@
         <v>127</v>
       </c>
       <c r="C21" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A21,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>AR</v>
       </c>
       <c r="D21" s="18"/>
@@ -7860,7 +7590,7 @@
         <v>128</v>
       </c>
       <c r="C22" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A22,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>AS</v>
       </c>
       <c r="D22" s="18"/>
@@ -7873,7 +7603,7 @@
         <v>129</v>
       </c>
       <c r="C23" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A23,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>AT</v>
       </c>
       <c r="D23" s="18"/>
@@ -7886,7 +7616,7 @@
         <v>130</v>
       </c>
       <c r="C24" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A24,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>AU</v>
       </c>
       <c r="D24" s="18"/>
@@ -7899,7 +7629,7 @@
         <v>131</v>
       </c>
       <c r="C25" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A25,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>C</v>
       </c>
       <c r="D25" s="18" t="s">
@@ -7914,7 +7644,7 @@
         <v>133</v>
       </c>
       <c r="C26" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A26,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BG</v>
       </c>
       <c r="D26" s="18"/>
@@ -7927,7 +7657,7 @@
         <v>134</v>
       </c>
       <c r="C27" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A27,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BH</v>
       </c>
       <c r="D27" s="18"/>
@@ -7940,7 +7670,7 @@
         <v>135</v>
       </c>
       <c r="C28" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A28,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BI</v>
       </c>
       <c r="D28" s="18"/>
@@ -7953,7 +7683,7 @@
         <v>136</v>
       </c>
       <c r="C29" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A29,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BJ</v>
       </c>
       <c r="D29" s="18"/>
@@ -7966,7 +7696,7 @@
         <v>137</v>
       </c>
       <c r="C30" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A30,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BK</v>
       </c>
       <c r="D30" s="18"/>
@@ -7979,7 +7709,7 @@
         <v>138</v>
       </c>
       <c r="C31" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A31,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BL</v>
       </c>
       <c r="D31" s="18"/>
@@ -7992,7 +7722,7 @@
         <v>139</v>
       </c>
       <c r="C32" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A32,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BM</v>
       </c>
       <c r="D32" s="18"/>
@@ -8005,7 +7735,7 @@
         <v>140</v>
       </c>
       <c r="C33" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A33,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BN</v>
       </c>
       <c r="D33" s="18"/>
@@ -8018,7 +7748,7 @@
         <v>141</v>
       </c>
       <c r="C34" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A34,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BO</v>
       </c>
       <c r="D34" s="18"/>
@@ -8031,7 +7761,7 @@
         <v>148</v>
       </c>
       <c r="C35" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A35,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BP</v>
       </c>
       <c r="D35" s="18"/>
@@ -8044,7 +7774,7 @@
         <v>149</v>
       </c>
       <c r="C36" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A36,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BQ</v>
       </c>
       <c r="D36" s="18"/>
@@ -8057,7 +7787,7 @@
         <v>150</v>
       </c>
       <c r="C37" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A37,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BR</v>
       </c>
       <c r="D37" s="18"/>
@@ -8070,7 +7800,7 @@
         <v>151</v>
       </c>
       <c r="C38" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A38,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BS</v>
       </c>
       <c r="D38" s="18"/>
@@ -8083,7 +7813,7 @@
         <v>152</v>
       </c>
       <c r="C39" s="18" t="str">
-        <f ca="1">SUBSTITUTE(ADDRESS(1,_xlfn.XMATCH(A39,[1]ИсходныеДанные!$A$1:$DD$1,0,1),4),1,"")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>BT</v>
       </c>
       <c r="D39" s="18"/>

</xml_diff>